<commit_message>
Creazione delle tabelle nella pagina Calendario. Creazione e gestione dei bottoni di switching, manca la parte grafica.
</commit_message>
<xml_diff>
--- a/organization/Organizzazione - GoalTrackr.xlsx
+++ b/organization/Organizzazione - GoalTrackr.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
   <si>
     <t>Task</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Note</t>
-  </si>
-  <si>
-    <t>Indirizzamento pagine esistenti fatto, manca la creazione e la gestione di alcune pagine.</t>
   </si>
   <si>
     <t>Creazione effettuata, creazione delle collezioni coaches e players con dati di esempio.
@@ -83,13 +80,105 @@
   </si>
   <si>
     <t>Vedere google e facebook authentication e decidere se rimuoverle.</t>
+  </si>
+  <si>
+    <t>Gestione della presenza attraverso una specie di tabella che indichi 
+gli eventi nella data corrente con affianco 2 bottoni.</t>
+  </si>
+  <si>
+    <t>Indirizzamento pagine esistenti fatto, manca la creazione e la gestione 
+di alcune pagine.</t>
+  </si>
+  <si>
+    <t>DETTAGLIO</t>
+  </si>
+  <si>
+    <t>Bottone PRESENTE: Segna la presenza ad un evento</t>
+  </si>
+  <si>
+    <t>I bottoni sono attivi solo fino a un'ora prima dell'inizio dell'evento</t>
+  </si>
+  <si>
+    <t>Pagina organizzazione eventi (allenatore)</t>
+  </si>
+  <si>
+    <t>Una tabella settimanale con gli eventi per ogni giorno e l'orario dell'evento.</t>
+  </si>
+  <si>
+    <t>Click sull'evento per modificarlo o eliminarlo.</t>
+  </si>
+  <si>
+    <t>Pagina presenze (giocatore)</t>
+  </si>
+  <si>
+    <t>Pagina eventi (giocatore)</t>
+  </si>
+  <si>
+    <t>Click sull'evento per segnalare la propria presenza o assenza in anticipo.</t>
+  </si>
+  <si>
+    <t>Pagina giocatori</t>
+  </si>
+  <si>
+    <t>Una tabella con l'elenco dei giocatori della squadra e le loro specifiche.</t>
+  </si>
+  <si>
+    <t>Pagina squadra</t>
+  </si>
+  <si>
+    <t>Specifiche sulla squadra (es. nome, campo di gioco, numero di giocatori, allenatore e staff…)</t>
+  </si>
+  <si>
+    <t>Statistiche giocatori</t>
+  </si>
+  <si>
+    <t>Una tabella con statistiche per ogni giocatore (es. partite giocate, gol, assist, cartellini…)</t>
+  </si>
+  <si>
+    <t>Statistiche giocatori (allenatore)</t>
+  </si>
+  <si>
+    <t>Possibilità di aggiungere dei dati ai giocatori</t>
+  </si>
+  <si>
+    <t>Bottone ASSENTE: Segna la non presenza ad un evento. Apre una Swal con una lista in cui si può scegliere la motivazione per l'assenza.</t>
+  </si>
+  <si>
+    <t>Gestione dei valori della tabella in base ai dati del database</t>
+  </si>
+  <si>
+    <t>Pagina calendario (giocatore)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creazione delle prime funzioni di gestione dei toggle e dei bottoni 
+di presenza e assenza. Inizio della gestione di switching tra programma
+generale e visualizzazione dettagliata degli eventi. </t>
+  </si>
+  <si>
+    <t>Come calendario, ma specifica per le singole categorie di eventi.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Una tabella settimanale con gli eventi per ogni giorno e l'orario dell'evento. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Da gestire i bottoni</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,8 +216,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="17"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,8 +278,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -189,11 +308,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -228,11 +384,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -519,36 +711,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="47.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="92.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.77734375" customWidth="1"/>
     <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -569,7 +761,7 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="15" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3"/>
@@ -584,12 +776,12 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:6" ht="108" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="7">
         <v>45338</v>
@@ -600,11 +792,11 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="15" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -613,44 +805,50 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="13"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="11"/>
+      <c r="B8" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="7">
+        <v>45354</v>
+      </c>
       <c r="D8" s="11"/>
-      <c r="E8" s="10" t="s">
-        <v>10</v>
+      <c r="E8" s="9" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="11"/>
+      <c r="C9" s="7">
+        <v>45354</v>
+      </c>
       <c r="D9" s="11"/>
-      <c r="E9" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="E9" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="36" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>16</v>
+      <c r="B10" s="14" t="s">
+        <v>19</v>
       </c>
       <c r="C10" s="7">
         <v>45338</v>
@@ -660,9 +858,198 @@
         <v>8</v>
       </c>
     </row>
+    <row r="11" spans="1:6" ht="22.2" x14ac:dyDescent="0.45">
+      <c r="A11" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="19"/>
+    </row>
+    <row r="12" spans="1:6" ht="36" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="21"/>
+      <c r="E12" s="22"/>
+    </row>
+    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A13" s="13"/>
+      <c r="B13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22"/>
+    </row>
+    <row r="14" spans="1:6" ht="36" x14ac:dyDescent="0.3">
+      <c r="A14" s="13"/>
+      <c r="B14" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="22"/>
+    </row>
+    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A15" s="13"/>
+      <c r="B15" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+    </row>
+    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A16" s="13"/>
+      <c r="B16" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+    </row>
+    <row r="17" spans="1:5" ht="36" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+    </row>
+    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="B18" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+    </row>
+    <row r="19" spans="1:5" ht="36" x14ac:dyDescent="0.3">
+      <c r="A19" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="24"/>
+      <c r="E19" s="25"/>
+    </row>
+    <row r="20" spans="1:5" ht="36" x14ac:dyDescent="0.3">
+      <c r="B20" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+    </row>
+    <row r="21" spans="1:5" ht="36" x14ac:dyDescent="0.3">
+      <c r="A21" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+    </row>
+    <row r="22" spans="1:5" ht="36" x14ac:dyDescent="0.3">
+      <c r="A22" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+    </row>
+    <row r="23" spans="1:5" ht="36" x14ac:dyDescent="0.3">
+      <c r="A23" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+    </row>
+    <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A24" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+    </row>
+    <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A25" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="16">
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
     <mergeCell ref="A1:E2"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Creazione servizio getGiocatori per inserire i giocatori della squadra nella tabella della pagina Giocatori. Gestione dell'ordinamento per campo nelle tabelle
</commit_message>
<xml_diff>
--- a/organization/Organizzazione - GoalTrackr.xlsx
+++ b/organization/Organizzazione - GoalTrackr.xlsx
@@ -120,9 +120,6 @@
     <t>Pagina giocatori</t>
   </si>
   <si>
-    <t>Una tabella con l'elenco dei giocatori della squadra e le loro specifiche.</t>
-  </si>
-  <si>
     <t>Pagina squadra</t>
   </si>
   <si>
@@ -148,11 +145,6 @@
   </si>
   <si>
     <t>Pagina calendario (giocatore)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creazione delle prime funzioni di gestione dei toggle e dei bottoni 
-di presenza e assenza. Inizio della gestione di switching tra programma
-generale e visualizzazione dettagliata degli eventi. </t>
   </si>
   <si>
     <t>Come calendario, ma specifica per le singole categorie di eventi.</t>
@@ -172,6 +164,16 @@
       </rPr>
       <t>Da gestire i bottoni</t>
     </r>
+  </si>
+  <si>
+    <t>Creazione delle prime funzioni di gestione dei toggle e dei bottoni 
+di presenza e assenza. Inizio della gestione di switching tra programma
+generale e visualizzazione dettagliata degli eventi. 
+Creata funzione per richiedere i giocatori. Da fare per squadra.</t>
+  </si>
+  <si>
+    <t>Una tabella con l'elenco dei giocatori della squadra e le loro specifiche.
+Per ogni giocatore c'è un button "Visualizza statistiche" che porta alla pagina statistiche giocatori.</t>
   </si>
 </sst>
 </file>
@@ -402,6 +404,15 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -415,15 +426,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -713,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -727,20 +729,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
     </row>
     <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -809,18 +811,20 @@
         <v>11</v>
       </c>
       <c r="B7" s="12"/>
-      <c r="C7" s="11"/>
+      <c r="C7" s="7">
+        <v>45359</v>
+      </c>
       <c r="D7" s="11"/>
-      <c r="E7" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="E7" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C8" s="7">
         <v>45354</v>
@@ -859,10 +863,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="22.2" x14ac:dyDescent="0.45">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="19"/>
+      <c r="B11" s="22"/>
     </row>
     <row r="12" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
@@ -871,38 +875,38 @@
       <c r="B12" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="22"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="25"/>
     </row>
     <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
       <c r="B13" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="22"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="25"/>
     </row>
     <row r="14" spans="1:6" ht="36" x14ac:dyDescent="0.3">
       <c r="A14" s="13"/>
       <c r="B14" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="22"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="25"/>
     </row>
     <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A15" s="13"/>
       <c r="B15" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>10</v>
@@ -946,16 +950,16 @@
     </row>
     <row r="19" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="20"/>
     </row>
     <row r="20" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="B20" s="14" t="s">
@@ -967,25 +971,25 @@
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
     </row>
-    <row r="21" spans="1:5" ht="36" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
         <v>29</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
+        <v>42</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="19"/>
+      <c r="E21" s="20"/>
     </row>
     <row r="22" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="14" t="s">
         <v>31</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>32</v>
       </c>
       <c r="C22" s="17" t="s">
         <v>10</v>
@@ -995,10 +999,10 @@
     </row>
     <row r="23" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="14" t="s">
         <v>33</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>34</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>10</v>
@@ -1008,10 +1012,10 @@
     </row>
     <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="14" t="s">
         <v>35</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>36</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>10</v>
@@ -1024,7 +1028,7 @@
         <v>27</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>10</v>
@@ -1034,13 +1038,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="C18:E18"/>
@@ -1050,6 +1047,13 @@
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>